<commit_message>
Cải tiên quy trình
</commit_message>
<xml_diff>
--- a/docs/caancom-templates.xlsx
+++ b/docs/caancom-templates.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ZDungHDD\My Programming\Webs Php Projects\caancom4\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB1E2A0-7AE8-4F13-BC7B-84993C942269}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478749C4-A979-4D59-B035-238B3F19637B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Career-job-page" sheetId="1" r:id="rId1"/>
     <sheet name="Mục-Quy Trình" sheetId="4" r:id="rId2"/>
-    <sheet name="home" sheetId="2" r:id="rId3"/>
-    <sheet name="fields chung" sheetId="3" r:id="rId4"/>
+    <sheet name="Mục-phòng ban" sheetId="5" r:id="rId3"/>
+    <sheet name="home" sheetId="2" r:id="rId4"/>
+    <sheet name="fields chung" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
   <si>
     <t>Tên</t>
   </si>
@@ -90,25 +91,58 @@
     <t>Template đề nghị</t>
   </si>
   <si>
-    <t>Danh mục</t>
+    <t>dept-chung</t>
   </si>
   <si>
-    <t>Quy trình S</t>
+    <t>dept-marketing</t>
   </si>
   <si>
-    <t>Quy Trình</t>
+    <t>dept-sales</t>
   </si>
   <si>
-    <t>Tags</t>
+    <t>dept-admin</t>
   </si>
   <si>
-    <t>Tag</t>
+    <t>dept-hr</t>
   </si>
   <si>
-    <t>Chỉ nằm trong danh mục</t>
+    <t>Diễn giải</t>
   </si>
   <si>
-    <t>chỉ nằm trong tags</t>
+    <t>PHòng ban chung chung</t>
+  </si>
+  <si>
+    <t>Cho marketing</t>
+  </si>
+  <si>
+    <t>Cho salé</t>
+  </si>
+  <si>
+    <t>wkpr-chung</t>
+  </si>
+  <si>
+    <t>wkpr-marketing</t>
+  </si>
+  <si>
+    <t>wkpr-sales</t>
+  </si>
+  <si>
+    <t>wkpr-admin</t>
+  </si>
+  <si>
+    <t>wkpr-hr</t>
+  </si>
+  <si>
+    <t>wkpr-procedure</t>
+  </si>
+  <si>
+    <t>wkpr-tags</t>
+  </si>
+  <si>
+    <t>wkpr-tag</t>
+  </si>
+  <si>
+    <t>…..</t>
   </si>
 </sst>
 </file>
@@ -3401,16 +3435,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3433,6 +3467,92 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Hộp Văn bản 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC835E34-CB45-4E8C-956A-7FEA7BF0BAB9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="228600" y="247650"/>
+          <a:ext cx="3476625" cy="1752600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-SG" sz="1100"/>
+            <a:t>Nhân</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-SG" sz="1100" baseline="0"/>
+            <a:t> viên đăng nhập vào xem các quy trình, họ chỉ xem được cac quy trình thuộc phòng ban của họ mà thôi.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-SG" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-SG" sz="1100" baseline="0"/>
+            <a:t>Quy trình có nhiều tags để tiện phân danh mục.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-SG" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3766,51 +3886,78 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9695F0CF-2020-40BC-895D-61B68CBDB32A}">
-  <dimension ref="J4:L9"/>
+  <dimension ref="Q1:S13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1:U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="11" max="11" width="12.85546875" customWidth="1"/>
+    <col min="18" max="18" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="J4" t="s">
+    <row r="1" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q1" t="s">
         <v>19</v>
       </c>
+      <c r="S1" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="5" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="K5" t="s">
-        <v>21</v>
+    <row r="2" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="R2" t="s">
+        <v>29</v>
+      </c>
+      <c r="S2" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="6" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="K6" t="s">
-        <v>20</v>
+    <row r="3" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="R3" t="s">
+        <v>30</v>
+      </c>
+      <c r="S3" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="7" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="K7" t="s">
-        <v>22</v>
-      </c>
-      <c r="L7" t="s">
-        <v>25</v>
+    <row r="4" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="R4" t="s">
+        <v>31</v>
+      </c>
+      <c r="S4" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="8" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="K8" t="s">
-        <v>23</v>
+    <row r="5" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="R5" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="9" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="K9" t="s">
-        <v>24</v>
-      </c>
-      <c r="L9" t="s">
-        <v>26</v>
+    <row r="6" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="R6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="R7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="R11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="R12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="R13" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -3820,6 +3967,66 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5C15405-BA87-44E0-896F-648E73706BE4}">
+  <dimension ref="Q1:S6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R17" sqref="R17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="18" max="18" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="R2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="R3" t="s">
+        <v>21</v>
+      </c>
+      <c r="S3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="R4" t="s">
+        <v>22</v>
+      </c>
+      <c r="S4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="R5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="R6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0721863-45F0-43E8-A28D-AACA9A773602}">
   <dimension ref="O3:R5"/>
   <sheetViews>
@@ -3867,7 +4074,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C41FC0E2-8A12-4445-9E96-4A1492AB5941}">
   <dimension ref="A2:D3"/>
   <sheetViews>

</xml_diff>